<commit_message>
New test cases and workload for june
</commit_message>
<xml_diff>
--- a/docs/research/test_cases.xlsx
+++ b/docs/research/test_cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NOPLEX\Documents\GitHub\SEMs\docs\research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBAD9DF-83D9-43AB-B4FF-7B32C60D642C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC206C5-D1C2-4702-99B3-643E6CF5E04C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="2" sheetId="5" r:id="rId3"/>
     <sheet name="3" sheetId="6" r:id="rId4"/>
     <sheet name="4" sheetId="7" r:id="rId5"/>
+    <sheet name="5" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -573,19 +574,108 @@
     <t xml:space="preserve">Most likely, the outcome of this test wil be that precision has a linear proportion with the dataset size. In addition, the time will be afected with the dataset size, meaning, bigger dataset takes more time to train. </t>
   </si>
   <si>
-    <t>Comparison between original and 2x augmentation</t>
-  </si>
-  <si>
-    <t>Comparison between original and 5x augmentation</t>
-  </si>
-  <si>
-    <t>Comparison between original and 10x augmentation</t>
-  </si>
-  <si>
-    <t>Comparison between original and 50x augmentation</t>
-  </si>
-  <si>
-    <t>Comparison between original and 100x augmentation</t>
+    <t>Original dataset</t>
+  </si>
+  <si>
+    <t>2x Augmentation</t>
+  </si>
+  <si>
+    <t>5x Augmentation</t>
+  </si>
+  <si>
+    <t>10x Augmentation</t>
+  </si>
+  <si>
+    <t>50x Augmentation</t>
+  </si>
+  <si>
+    <t>Platform</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">For the test was used the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>version 1.0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of the platform </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Smart Energy Monitoring</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> as well as the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>prototype</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sensor for simulation real environment.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Conclude if the prototype has the same results in real environments as it did in a laboratory environment. </t>
+  </si>
+  <si>
+    <t>Create an account, setup the prototype with the account created, access the platform to finalize the initial configuration, make individual reads and start using it normally.</t>
+  </si>
+  <si>
+    <t>Is expected that the initial performance of the model won't be as good as it could be, but after some training it will get better. The platform will be easy to use and friendly to newcomers.</t>
+  </si>
+  <si>
+    <t>House A</t>
+  </si>
+  <si>
+    <t>House B</t>
+  </si>
+  <si>
+    <t>House C</t>
   </si>
 </sst>
 </file>
@@ -749,34 +839,16 @@
   </cellStyleXfs>
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -788,7 +860,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -804,6 +875,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1018,6 +1110,55 @@
         <a:xfrm>
           <a:off x="1504951" y="6467475"/>
           <a:ext cx="914400" cy="1092819"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2350233</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1971675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagem 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCE76AF9-DD81-4E58-8087-20C04621D899}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="7697" t="6171" r="7635" b="8899"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="838200" y="7991475"/>
+          <a:ext cx="2283558" cy="1619250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1292,10 +1433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1310,259 +1451,311 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="10" t="s">
+      <c r="B5" s="20"/>
+      <c r="C5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="23"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9" t="s">
+      <c r="B6" s="20"/>
+      <c r="C6" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9" t="s">
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="F9" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14">
+      <c r="A10" s="8">
         <v>1</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D10" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="19"/>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
+      <c r="A11" s="8">
         <v>2</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="4"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14">
+      <c r="A12" s="8">
         <v>3</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="23" t="s">
+      <c r="F12" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="4"/>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14">
+      <c r="A13" s="8">
         <v>4</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="23" t="s">
+      <c r="F13" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" ht="198" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" ht="156.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
         <v>5</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" ht="183.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14">
-        <v>6</v>
-      </c>
+      <c r="B14" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="24"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="18"/>
+      <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" ht="166.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14">
-        <v>7</v>
-      </c>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="24"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="18"/>
+      <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="1:7" ht="148.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14">
-        <v>8</v>
-      </c>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="24"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="18"/>
+      <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="1:7" ht="183" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14">
-        <v>9</v>
-      </c>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="24"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="18"/>
+      <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="1:7" ht="168.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14">
-        <v>10</v>
-      </c>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="24"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="18"/>
+      <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="4"/>
-    </row>
-    <row r="20" spans="1:7" ht="208.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14">
-        <v>11</v>
-      </c>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="24"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="18"/>
+      <c r="E20" s="3"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="4"/>
-    </row>
-    <row r="21" spans="1:7" ht="210" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14">
-        <v>12</v>
-      </c>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="24"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="18"/>
+      <c r="E21" s="3"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="4"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1595,52 +1788,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="18"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>3</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>4</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1657,7 +1850,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1667,46 +1860,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="18"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1721,7 +1914,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1731,52 +1924,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="18"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>3</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>4</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1793,7 +1986,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q28" sqref="Q28:Q29"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1803,65 +1996,140 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="18"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>3</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>4</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>5</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="23" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D23" s="2"/>
+      <c r="D23" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{426BF2A1-97E6-4ED3-B072-0990C54EC85F}">
+  <dimension ref="A1:D23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="74.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="18"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
3D models and test cases
</commit_message>
<xml_diff>
--- a/docs/research/test_cases.xlsx
+++ b/docs/research/test_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NOPLEX\Documents\GitHub\SEMs\docs\research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepository\SEM\docs\research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC206C5-D1C2-4702-99B3-643E6CF5E04C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B450C6A-3C4D-44FF-81BC-E893C58C09F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="78">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -529,18 +529,6 @@
     </r>
   </si>
   <si>
-    <t>Calibration with "EmonLib.h" in house A</t>
-  </si>
-  <si>
-    <t>Calibration with formula in house A</t>
-  </si>
-  <si>
-    <t>Calibration with "EmonLib.h" in house B</t>
-  </si>
-  <si>
-    <t>Calibration with formula in house B</t>
-  </si>
-  <si>
     <t>Find how many examples are enough to have a relatively optimal model. Find if data augmentation is really required in this case. Comparation between training time and the dataset size.</t>
   </si>
   <si>
@@ -669,13 +657,85 @@
     <t>Is expected that the initial performance of the model won't be as good as it could be, but after some training it will get better. The platform will be easy to use and friendly to newcomers.</t>
   </si>
   <si>
-    <t>House A</t>
-  </si>
-  <si>
-    <t>House B</t>
-  </si>
-  <si>
-    <t>House C</t>
+    <t>Add equipment - Save to database</t>
+  </si>
+  <si>
+    <t>Add division - Save to database</t>
+  </si>
+  <si>
+    <t>Add affiliate - Save to database</t>
+  </si>
+  <si>
+    <t>Dynamic update between pages (Websockets - "equipmentUpdate" call )</t>
+  </si>
+  <si>
+    <t>Dynamic update between pages (Websockets - "divisionUpdate" call )</t>
+  </si>
+  <si>
+    <t>Dynamic update between pages (Websockets - "affiliateUpdate" call )</t>
+  </si>
+  <si>
+    <t>Check required fields on form submit - Add division</t>
+  </si>
+  <si>
+    <t>Check required fields on form submit - Add affiliate</t>
+  </si>
+  <si>
+    <t>Check required fields on form submit - Edit Profile</t>
+  </si>
+  <si>
+    <t>Dynamic update between pages (Websockets - "profileUpdate" call )</t>
+  </si>
+  <si>
+    <t>Edit Profile - Save to database</t>
+  </si>
+  <si>
+    <t>Check required fields on form submit - Change Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change password </t>
+  </si>
+  <si>
+    <t>Check notifications for each expriment</t>
+  </si>
+  <si>
+    <t>Register - Check user created</t>
+  </si>
+  <si>
+    <t>Register - Redirect to dashboard after auto login</t>
+  </si>
+  <si>
+    <t>Edit equipment - Save to database</t>
+  </si>
+  <si>
+    <t>Check required fields on form submit - equipment</t>
+  </si>
+  <si>
+    <t>Delete equipment</t>
+  </si>
+  <si>
+    <t>Edit division - Save to database</t>
+  </si>
+  <si>
+    <t>Delete division</t>
+  </si>
+  <si>
+    <t>Delete affiliate</t>
+  </si>
+  <si>
+    <t>Check train examples - save to database</t>
+  </si>
+  <si>
+    <t>Try to add an affiliate that is not on the system</t>
+  </si>
+  <si>
+    <t>Check if the user only has access to the right information</t>
+  </si>
+  <si>
+    <t>Calibration with "EmonLib.h"</t>
+  </si>
+  <si>
+    <t>Calibration with formula</t>
   </si>
 </sst>
 </file>
@@ -714,7 +774,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -729,6 +789,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -837,7 +909,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -876,6 +948,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -893,9 +970,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -921,13 +995,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>819151</xdr:colOff>
+      <xdr:colOff>657226</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>314325</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1552576</xdr:colOff>
+      <xdr:colOff>1390651</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>1047750</xdr:rowOff>
     </xdr:to>
@@ -958,7 +1032,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1590676" y="2028825"/>
+          <a:off x="1428751" y="2028825"/>
           <a:ext cx="733425" cy="733425"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1435,8 +1509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1451,60 +1525,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21" t="s">
+      <c r="B5" s="23"/>
+      <c r="C5" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="23"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="26"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20" t="s">
+      <c r="B6" s="23"/>
+      <c r="C6" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20" t="s">
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
@@ -1518,7 +1592,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>1</v>
@@ -1544,7 +1618,7 @@
         <v>12</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E10" s="16" t="s">
         <v>18</v>
@@ -1607,13 +1681,13 @@
         <v>29</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G13" s="3"/>
     </row>
@@ -1622,24 +1696,24 @@
         <v>5</v>
       </c>
       <c r="B14" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>54</v>
-      </c>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -1648,7 +1722,7 @@
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -1657,7 +1731,7 @@
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -1666,7 +1740,7 @@
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1675,7 +1749,7 @@
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -1684,7 +1758,7 @@
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
+      <c r="A20" s="18"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -1693,7 +1767,7 @@
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="24"/>
+      <c r="A21" s="18"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -1777,8 +1851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49793489-8A56-4CDB-AC41-B339307EE88A}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1788,14 +1862,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="18"/>
+      <c r="B1" s="21"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1810,7 +1884,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1818,24 +1892,16 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>31</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>3</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>4</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>33</v>
-      </c>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1850,7 +1916,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1860,14 +1926,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="18"/>
+      <c r="B1" s="21"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1882,7 +1948,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1890,7 +1956,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1924,14 +1990,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="18"/>
+      <c r="B1" s="21"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1946,7 +2012,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1954,7 +2020,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1962,7 +2028,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1970,7 +2036,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1986,7 +2052,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1996,14 +2062,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="18"/>
+      <c r="B1" s="21"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -2018,7 +2084,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2026,7 +2092,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2034,7 +2100,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2042,7 +2108,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2050,7 +2116,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="4:4" x14ac:dyDescent="0.25">
@@ -2066,10 +2132,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{426BF2A1-97E6-4ED3-B072-0990C54EC85F}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2079,14 +2145,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" s="18"/>
+      <c r="A1" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="21"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -2100,41 +2166,214 @@
       <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>55</v>
+      <c r="B5" s="19" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>56</v>
+      <c r="B6" s="19" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>3</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>4</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>5</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>6</v>
+      </c>
+      <c r="B10" s="20" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-    </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>8</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>9</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>10</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>11</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>12</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>13</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>14</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>15</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>16</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>17</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>18</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>19</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>20</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>62</v>
+      </c>
       <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>21</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>22</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>23</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>24</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>25</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>26</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>